<commit_message>
Test Cases For Flipkart Excel
</commit_message>
<xml_diff>
--- a/Flipkart.xlsx
+++ b/Flipkart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="123">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -456,12 +456,54 @@
 Reopen the browser or revisit the Flipkart website.
 Verify that the user is automatically logged in without having to re-enter the credentials.</t>
   </si>
+  <si>
+    <t>To Verify that a registered user can log in 
+with valid credentials.</t>
+  </si>
+  <si>
+    <t>Precondition</t>
+  </si>
+  <si>
+    <t>Flipkart page should be Open after entering URL</t>
+  </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t>https://www.flipkart.com/</t>
+  </si>
+  <si>
+    <t>Login ID - vvnjiks@gmail.com
+Mobile Number- 8776985877</t>
+  </si>
+  <si>
+    <t>Login Page should be open successfully</t>
+  </si>
+  <si>
+    <t>Login page Opened Successfully</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Flipkart page should be Open with Login Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> To Verify that an error message is displayed for 
+incorrect login credentials.</t>
+  </si>
+  <si>
+    <t>User should Login Successfully.</t>
+  </si>
+  <si>
+    <t>User able to Login Successfully</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,6 +513,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -514,10 +572,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -528,8 +587,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -829,10 +892,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,14 +903,15 @@
     <col min="1" max="1" width="41.5703125" style="4" customWidth="1"/>
     <col min="2" max="3" width="14.5703125" style="4" customWidth="1"/>
     <col min="4" max="4" width="97.140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="37.140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="109.140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="4"/>
+    <col min="5" max="5" width="63.85546875" style="4" customWidth="1"/>
+    <col min="6" max="7" width="46.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="109.140625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="35.140625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="30" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -864,19 +928,25 @@
         <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -892,77 +962,119 @@
       <c r="E2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="I2" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>98</v>
       </c>
+      <c r="E3" s="5" t="s">
+        <v>110</v>
+      </c>
       <c r="F3" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="I3" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="C4" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="E4" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="C7" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="H8" s="5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
@@ -976,7 +1088,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
@@ -984,7 +1096,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C12" s="4" t="s">
         <v>13</v>
       </c>
@@ -992,7 +1104,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C13" s="4" t="s">
         <v>14</v>
       </c>
@@ -1000,7 +1112,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="C14" s="4" t="s">
         <v>15</v>
       </c>
@@ -1008,7 +1120,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C15" s="4" t="s">
         <v>16</v>
       </c>
@@ -1016,7 +1128,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C16" s="4" t="s">
         <v>41</v>
       </c>
@@ -1024,7 +1136,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C17" s="4" t="s">
         <v>42</v>
       </c>
@@ -1032,7 +1144,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C18" s="4" t="s">
         <v>43</v>
       </c>
@@ -1040,7 +1152,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C19" s="4" t="s">
         <v>44</v>
       </c>
@@ -1048,7 +1160,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C20" s="4" t="s">
         <v>45</v>
       </c>
@@ -1056,7 +1168,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C21" s="4" t="s">
         <v>46</v>
       </c>
@@ -1064,7 +1176,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C22" s="4" t="s">
         <v>47</v>
       </c>
@@ -1072,7 +1184,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C23" s="4" t="s">
         <v>48</v>
       </c>
@@ -1080,7 +1192,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C24" s="4" t="s">
         <v>49</v>
       </c>
@@ -1088,7 +1200,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>35</v>
       </c>
@@ -1101,58 +1213,62 @@
       <c r="D26" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="H26" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="C27" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="C28" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="H28" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="C29" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="H29" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="C30" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>56</v>
       </c>
@@ -1165,58 +1281,68 @@
       <c r="D32" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="C33" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="C34" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="C35" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="H35" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="C36" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>68</v>
       </c>
@@ -1229,55 +1355,61 @@
       <c r="D38" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="C39" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="C40" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="C41" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F41" s="5" t="s">
+      <c r="H41" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="C42" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F42" s="5" t="s">
+      <c r="H42" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>80</v>
       </c>
@@ -1290,79 +1422,82 @@
       <c r="D44" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="H44" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="C45" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F45" s="5" t="s">
+      <c r="H45" s="5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="C46" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F46" s="5" t="s">
+      <c r="H46" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="C47" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="F47" s="5" t="s">
+      <c r="H47" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="C48" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="F48" s="5" t="s">
+      <c r="H48" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="3:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:8" ht="75" x14ac:dyDescent="0.25">
       <c r="C49" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="F49" s="5" t="s">
+      <c r="H49" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="50" spans="3:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:8" ht="75" x14ac:dyDescent="0.25">
       <c r="C50" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="F50" s="5" t="s">
+      <c r="H50" s="5" t="s">
         <v>95</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>